<commit_message>
now output has chemical and bio inputs
</commit_message>
<xml_diff>
--- a/tests/Arnot_match _Pore_water_Dissolved_Water.xlsx
+++ b/tests/Arnot_match _Pore_water_Dissolved_Water.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_and_Time_Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="122">
   <si>
     <t xml:space="preserve">Sampling Variables Inputs</t>
   </si>
@@ -293,10 +293,19 @@
     <t xml:space="preserve">Fraction Pore Water Ventilated (deafult = 0)</t>
   </si>
   <si>
+    <t xml:space="preserve">Dietary absorption efficency of lipid Organic Matter (deafult  = .75)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dietary absorption efficency of lipid Organic Matter (deafult  = .72)</t>
   </si>
   <si>
+    <t xml:space="preserve">Dietary absorption efficency of nonlipid Organic Matter (deafult  = .75)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dietary absorption efficency of nonlipid Organic Matter (deafult  = .72)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dietary absorption efficency of water (deafult  = .5)</t>
   </si>
   <si>
     <t xml:space="preserve">Dietary absorption efficency of water (deafult  = .25)</t>
@@ -1157,9 +1166,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1018080</xdr:colOff>
+      <xdr:colOff>1017720</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1169,7 +1178,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14044680" y="863280"/>
-          <a:ext cx="9470520" cy="7618320"/>
+          <a:ext cx="9470160" cy="7617960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1636,9 +1645,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3630240</xdr:colOff>
+      <xdr:colOff>3629880</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>182160</xdr:rowOff>
+      <xdr:rowOff>181800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1648,7 +1657,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12525120" y="699480"/>
-          <a:ext cx="3083760" cy="995040"/>
+          <a:ext cx="3083400" cy="994680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1859,9 +1868,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2330640</xdr:colOff>
+      <xdr:colOff>2330280</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1875,7 +1884,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16676280" y="10278720"/>
-          <a:ext cx="2330640" cy="734760"/>
+          <a:ext cx="2330280" cy="734400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1896,7 +1905,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4592160</xdr:colOff>
+      <xdr:colOff>4591800</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
@@ -1908,7 +1917,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11825640" y="2007000"/>
-          <a:ext cx="9442800" cy="3200760"/>
+          <a:ext cx="9442440" cy="3200760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2375,9 +2384,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>785520</xdr:colOff>
+      <xdr:colOff>785160</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>189000</xdr:rowOff>
+      <xdr:rowOff>188640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2387,7 +2396,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16928640" y="190440"/>
-          <a:ext cx="3602520" cy="760320"/>
+          <a:ext cx="3602160" cy="759960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2517,9 +2526,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1132200</xdr:colOff>
+      <xdr:colOff>1131840</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2529,7 +2538,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14774760" y="1714680"/>
-          <a:ext cx="2930040" cy="759960"/>
+          <a:ext cx="2929680" cy="759600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2601,9 +2610,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>642960</xdr:colOff>
+      <xdr:colOff>642600</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2613,7 +2622,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10537200" y="2522160"/>
-          <a:ext cx="9087480" cy="3567240"/>
+          <a:ext cx="9087120" cy="3566880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3141,9 +3150,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>150480</xdr:colOff>
+      <xdr:colOff>150120</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3153,7 +3162,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10606320" y="674280"/>
-          <a:ext cx="4074840" cy="948600"/>
+          <a:ext cx="4074480" cy="948240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3260,9 +3269,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3565800</xdr:colOff>
+      <xdr:colOff>3565440</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>45360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3272,7 +3281,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4629240" y="4925160"/>
-          <a:ext cx="5157360" cy="760320"/>
+          <a:ext cx="5157000" cy="759960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3374,9 +3383,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2592360</xdr:colOff>
+      <xdr:colOff>2592000</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>189360</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3386,7 +3395,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16049880" y="5488560"/>
-          <a:ext cx="4330440" cy="340560"/>
+          <a:ext cx="4330080" cy="340200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3458,9 +3467,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5383080</xdr:colOff>
+      <xdr:colOff>5382720</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:rowOff>137520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3470,7 +3479,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9213840" y="76320"/>
-          <a:ext cx="5256000" cy="1496520"/>
+          <a:ext cx="5255640" cy="1496160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3672,9 +3681,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6883560</xdr:colOff>
+      <xdr:colOff>6883200</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3684,7 +3693,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10153440" y="2298600"/>
-          <a:ext cx="5816880" cy="658440"/>
+          <a:ext cx="5816520" cy="658080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3791,9 +3800,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>252360</xdr:colOff>
+      <xdr:colOff>252000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3803,7 +3812,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11960640" y="241200"/>
-          <a:ext cx="5135400" cy="391680"/>
+          <a:ext cx="5135040" cy="391320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3915,9 +3924,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>99720</xdr:colOff>
+      <xdr:colOff>99360</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3927,7 +3936,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12062160" y="1295280"/>
-          <a:ext cx="3861720" cy="417240"/>
+          <a:ext cx="3861360" cy="416880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3984,9 +3993,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>468360</xdr:colOff>
+      <xdr:colOff>468000</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3996,7 +4005,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12087720" y="2158560"/>
-          <a:ext cx="5224320" cy="696960"/>
+          <a:ext cx="5223960" cy="696600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4058,9 +4067,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>277560</xdr:colOff>
+      <xdr:colOff>277200</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4070,7 +4079,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13899240" y="761760"/>
-          <a:ext cx="6530040" cy="5878440"/>
+          <a:ext cx="6529680" cy="5878080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4186,7 +4195,7 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -4944,8 +4953,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5107,54 +5116,54 @@
       </c>
       <c r="B7" s="52"/>
       <c r="C7" s="28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="53"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B8" s="52"/>
       <c r="C8" s="28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B9" s="49"/>
       <c r="C9" s="28" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="28" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B10" s="54"/>
       <c r="C10" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -5175,19 +5184,19 @@
     </row>
     <row r="12" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="56" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B12" s="55" t="n">
         <v>0</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D12" s="57" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F12" s="58" t="n">
         <v>0</v>
@@ -5216,7 +5225,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5261,7 +5270,7 @@
       <c r="A19" s="3"/>
       <c r="B19" s="18"/>
       <c r="C19" s="28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D19" s="12"/>
     </row>
@@ -5269,7 +5278,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="18"/>
       <c r="C20" s="28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D20" s="12"/>
     </row>
@@ -5277,7 +5286,7 @@
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="28" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D21" s="12"/>
     </row>
@@ -5285,7 +5294,7 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D22" s="12"/>
     </row>
@@ -5301,7 +5310,7 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="56" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D24" s="57" t="n">
         <v>0</v>
@@ -5348,7 +5357,7 @@
         <v>51</v>
       </c>
       <c r="B1" s="61" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5359,7 +5368,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="62" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B3" s="62" t="n">
         <v>0.4</v>
@@ -5391,7 +5400,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="62" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B7" s="62" t="n">
         <v>0</v>
@@ -5413,18 +5422,18 @@
         <v>51</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="62" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="62" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B11" s="62" t="n">
         <v>0.5</v>
@@ -5456,7 +5465,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="62" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B15" s="62" t="n">
         <v>0</v>
@@ -5478,7 +5487,7 @@
         <v>51</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5489,7 +5498,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="62" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B19" s="62" t="n">
         <v>0.05</v>
@@ -5521,7 +5530,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="62" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B23" s="62" t="n">
         <v>0.1</v>
@@ -5608,13 +5617,13 @@
         <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E1" s="18"/>
       <c r="TU1" s="0"/>
@@ -6104,7 +6113,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="63" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B2" s="64" t="n">
         <v>1</v>
@@ -6171,19 +6180,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -6192,16 +6201,16 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12"/>
       <c r="B2" s="12" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F2" s="32"/>
       <c r="G2" s="32"/>
@@ -6209,13 +6218,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
@@ -6229,7 +6238,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
@@ -6579,16 +6588,16 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="67" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B39" s="67" t="n">
         <v>40</v>
       </c>
       <c r="C39" s="67" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D39" s="67" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E39" s="32"/>
       <c r="F39" s="32"/>
@@ -6597,49 +6606,49 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B40" s="64" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C40" s="64" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D40" s="68" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E40" s="68" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F40" s="68" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G40" s="68" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="H40" s="69"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="64" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B41" s="64" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C41" s="64" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="64" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E41" s="64" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F41" s="64" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G41" s="64" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="H41" s="32"/>
       <c r="AW41" s="0" t="s">

</xml_diff>